<commit_message>
Investigate correlations of predictors and damages
</commit_message>
<xml_diff>
--- a/data/raw/economic-data.xlsx
+++ b/data/raw/economic-data.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10119"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="6" documentId="11_B2E4ED6710240B82ED5C7089507567A1A65D4467" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AFDB35A8-14DC-B248-AC8B-9A7516B822AD}"/>
+  <xr:revisionPtr revIDLastSave="9" documentId="11_B2E4ED6710240B82ED5C7089507567A1A65D4467" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5388958C-13B7-ED43-9E33-7853C7CFD74F}"/>
   <bookViews>
     <workbookView xWindow="4360" yWindow="2480" windowWidth="19800" windowHeight="14800" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -5470,10 +5470,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5736,7 +5732,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AT450"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="I4" workbookViewId="0">
       <selection activeCell="AP180" sqref="AP180"/>
     </sheetView>
   </sheetViews>
@@ -5745,6 +5741,7 @@
     <col min="5" max="5" width="44.33203125" customWidth="1"/>
     <col min="7" max="7" width="32.5" customWidth="1"/>
     <col min="9" max="9" width="19.5" customWidth="1"/>
+    <col min="16" max="16" width="32.6640625" customWidth="1"/>
     <col min="42" max="42" width="30.5" customWidth="1"/>
   </cols>
   <sheetData>

</xml_diff>